<commit_message>
ke: update Kenya forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Kenya/ke_lf_pretas_1_site_202203.xlsx
+++ b/LF/PreTAS/Kenya/ke_lf_pretas_1_site_202203.xlsx
@@ -70,7 +70,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>select_one enumarator</t>
+    <t>string</t>
   </si>
   <si>
     <t>c_enumerator</t>
@@ -79,7 +79,7 @@
     <t>Enumerator</t>
   </si>
   <si>
-    <t>Select your name/number</t>
+    <t>Write first and last name</t>
   </si>
   <si>
     <t>select_one county</t>
@@ -340,10 +340,10 @@
     <t xml:space="preserve">allow_choice_duplicates </t>
   </si>
   <si>
-    <t>1. Kenya - Pre TAS LF Site Form V2</t>
-  </si>
-  <si>
-    <t>ke_lf_pretas_1_site_202203_v2</t>
+    <t>1. Kenya - Pre TAS LF Site Form V3</t>
+  </si>
+  <si>
+    <t>ke_lf_pretas_1_site_202203_v3</t>
   </si>
   <si>
     <t>English</t>
@@ -363,9 +363,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
@@ -431,10 +431,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -453,6 +485,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -461,9 +500,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -486,7 +524,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,43 +538,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,9 +546,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,7 +561,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,7 +582,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,7 +612,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,19 +624,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,13 +684,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,43 +714,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,13 +732,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,49 +756,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,6 +806,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -830,11 +845,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -854,21 +875,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -876,21 +882,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -903,145 +894,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1421,11 +1421,11 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="$A13:$XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1737,7 +1737,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
@@ -2537,13 +2537,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="46.1259259259259" customWidth="1"/>
-    <col min="2" max="2" width="24.5037037037037" customWidth="1"/>
+    <col min="2" max="2" width="28.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="15.8740740740741" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>